<commit_message>
update the program of washing data, and cleaned dataset.
</commit_message>
<xml_diff>
--- a/data/countries.xlsx
+++ b/data/countries.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinhanmei/Desktop/liuyuzhou svm model playground/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinhanmei/Desktop/LME-and-CME-Essay/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F129CA6E-5834-D74C-92A3-6EC42083EEFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57F5AB1-E580-2D46-8B60-25AE8B09A0C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17040" yWindow="1840" windowWidth="21360" windowHeight="18620" xr2:uid="{58C66EA2-6E6C-2943-96CE-4856D3894EFC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Belgium</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Sweden</t>
   </si>
   <si>
-    <t>Witt and Jackson 2016</t>
-  </si>
-  <si>
     <t>LME</t>
   </si>
   <si>
@@ -93,6 +90,14 @@
   </si>
   <si>
     <t>United Kingdom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hahaha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -466,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7EB002-0A6A-4348-B56E-FA75286D1EE0}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -479,10 +484,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -490,15 +495,15 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -506,39 +511,39 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -546,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -554,7 +559,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -562,15 +567,15 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -578,7 +583,7 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -586,31 +591,36 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>